<commit_message>
Author        : Sidhi Mishra Story Name    : Login Module Task          : Updated burmt hour for task T-1 Files Added   : None Files modified: SidhiMishra.xlsx Files deleted : None
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/SidhiMishra.xlsx
+++ b/TeamDetails/TasksBreakDown/SidhiMishra.xlsx
@@ -2735,7 +2735,7 @@
   <dimension ref="A2:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2775,7 +2775,9 @@
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>14</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2785,7 +2787,9 @@
       <c r="E3" s="2">
         <v>3</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
       <c r="G3" s="2">
         <v>0</v>
       </c>

</xml_diff>